<commit_message>
Identificação de requisitos e casos de uso
</commit_message>
<xml_diff>
--- a/Requisitos e Casos de Uso.xlsx
+++ b/Requisitos e Casos de Uso.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="56">
   <si>
     <t>REQUISITOS DO SISTEMA</t>
   </si>
@@ -132,13 +132,70 @@
   </si>
   <si>
     <t>UC10</t>
+  </si>
+  <si>
+    <t>O SISTEMA CONTROLA A MOVIMENTAÇAO DE EQUIPAMENTO</t>
+  </si>
+  <si>
+    <t>OS EQUIPAMENTOS ESTAO DIVIDIDOS EM 7 CATEGORIAS</t>
+  </si>
+  <si>
+    <t>CADASTRAR EQUIPAMENTO DE HARDWARE</t>
+  </si>
+  <si>
+    <t>CONSULTAR HISTORICO DE EQUIPAMENTO</t>
+  </si>
+  <si>
+    <t>MANTER USUARIO</t>
+  </si>
+  <si>
+    <t>MANTER LOTAÇOES</t>
+  </si>
+  <si>
+    <t>GERAR FICHA DE MOVIMENTAÇAO DE EQUIPAMENTO</t>
+  </si>
+  <si>
+    <t>GERAR RELATÓRIOS</t>
+  </si>
+  <si>
+    <t>REGISTRAR NUMERO DE HORAS DA LAMPADA DO PROJETOR</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> EXISTE UM RESPONSÁVEL POR CADA LOTAÇAO</t>
+  </si>
+  <si>
+    <t>REGISTRAR MOVIMENTAÇAO DE EQUIPAMENTO</t>
+  </si>
+  <si>
+    <t>CADASTRAR EQUIPAMENTO</t>
+  </si>
+  <si>
+    <t>GERAR RELATORIOS</t>
+  </si>
+  <si>
+    <t>MANTER USUÁRIOS</t>
+  </si>
+  <si>
+    <t>GERAR FIMI</t>
+  </si>
+  <si>
+    <t>MASTER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MASTER, ASSISTENTE </t>
+  </si>
+  <si>
+    <t>MASTER, ANALISTA</t>
+  </si>
+  <si>
+    <t>MASTER, GERENTE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -178,6 +235,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -203,7 +268,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -229,6 +294,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -537,8 +605,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -564,78 +632,122 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="4"/>
+      <c r="B3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
+      <c r="B4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="4"/>
-      <c r="C5" s="5"/>
+      <c r="B5" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>48</v>
+      </c>
       <c r="D5" s="6"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
+      <c r="B6" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>49</v>
+      </c>
       <c r="D6" s="6"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="4"/>
-      <c r="C7" s="5"/>
+      <c r="B7" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>50</v>
+      </c>
       <c r="D7" s="6"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="4"/>
-      <c r="C8" s="5"/>
+      <c r="B8" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>42</v>
+      </c>
       <c r="D8" s="6"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="5"/>
+      <c r="B9" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>51</v>
+      </c>
       <c r="D9" s="5"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="5"/>
-      <c r="C10" s="4"/>
+      <c r="B10" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>49</v>
+      </c>
       <c r="D10" s="5"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="4"/>
-      <c r="C11" s="6"/>
+      <c r="B11" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>45</v>
+      </c>
       <c r="D11" s="6"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="4"/>
-      <c r="C12" s="6"/>
+      <c r="B12" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>42</v>
+      </c>
       <c r="D12" s="6"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -643,7 +755,7 @@
         <v>11</v>
       </c>
       <c r="B13" s="4"/>
-      <c r="C13" s="5"/>
+      <c r="C13" s="10"/>
       <c r="D13" s="6"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -747,75 +859,110 @@
       <c r="A27" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="B27" s="4"/>
+      <c r="B27" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C27" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
         <v>28</v>
       </c>
+      <c r="B28" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C28" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="B29" s="5"/>
+      <c r="B29" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C29" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="B30" s="4"/>
+      <c r="B30" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C30" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="B31" s="5"/>
+      <c r="B31" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C31" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="B32" s="5"/>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B32" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C32" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="7" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B33" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C33" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="B34" s="4"/>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="7" t="s">
         <v>35</v>
       </c>
       <c r="B35" s="6"/>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="B36" s="6"/>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B37" s="5"/>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B38" s="6"/>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B39" s="4"/>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B40" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Correções no Diagrama de Casos de Uso, Inclusão da versão inicial da Especificação do UC02 e inclusão da versão inicial do protótipo do sistema
</commit_message>
<xml_diff>
--- a/Requisitos e Casos de Uso.xlsx
+++ b/Requisitos e Casos de Uso.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="12240" windowHeight="8025"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="60">
   <si>
     <t>REQUISITOS DO SISTEMA</t>
   </si>
@@ -189,13 +189,25 @@
   </si>
   <si>
     <t>MASTER, GERENTE</t>
+  </si>
+  <si>
+    <t>O acesso ao sistema deverá ser controlado através de login e senha</t>
+  </si>
+  <si>
+    <t>MANTER USUÁRIOS                AUTENTICAR USUÁRIO</t>
+  </si>
+  <si>
+    <t>AUTENTICAR USUÁRIO</t>
+  </si>
+  <si>
+    <t>MASTER, ASSISTENTE, GERENTE, ANALISTA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -235,14 +247,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -268,7 +272,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -295,15 +299,18 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
-    <cellStyle name="Hiperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperlink" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperlink Visitado" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Hiperlink Visitado" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink seguido" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink seguido" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -391,7 +398,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -426,7 +432,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Escritório">
@@ -602,26 +607,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="7.42578125" customWidth="1"/>
     <col min="2" max="2" width="65" customWidth="1"/>
     <col min="3" max="3" width="35.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" ht="23.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" s="2" t="s">
         <v>13</v>
       </c>
@@ -632,7 +637,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="30">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
@@ -643,7 +648,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
@@ -654,7 +659,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4">
       <c r="A5" s="7" t="s">
         <v>3</v>
       </c>
@@ -666,7 +671,7 @@
       </c>
       <c r="D5" s="6"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4">
       <c r="A6" s="7" t="s">
         <v>4</v>
       </c>
@@ -678,7 +683,7 @@
       </c>
       <c r="D6" s="6"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="A7" s="7" t="s">
         <v>5</v>
       </c>
@@ -690,7 +695,7 @@
       </c>
       <c r="D7" s="6"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4">
       <c r="A8" s="7" t="s">
         <v>6</v>
       </c>
@@ -702,7 +707,7 @@
       </c>
       <c r="D8" s="6"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4">
       <c r="A9" s="7" t="s">
         <v>7</v>
       </c>
@@ -714,7 +719,7 @@
       </c>
       <c r="D9" s="5"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4">
       <c r="A10" s="7" t="s">
         <v>8</v>
       </c>
@@ -726,11 +731,11 @@
       </c>
       <c r="D10" s="5"/>
     </row>
-    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="7" t="s">
+    <row r="11" spans="1:4" ht="30">
+      <c r="A11" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="10" t="s">
         <v>45</v>
       </c>
       <c r="C11" s="4" t="s">
@@ -738,7 +743,7 @@
       </c>
       <c r="D11" s="6"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4">
       <c r="A12" s="7" t="s">
         <v>10</v>
       </c>
@@ -750,15 +755,19 @@
       </c>
       <c r="D12" s="6"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="7" t="s">
+    <row r="13" spans="1:4" ht="30">
+      <c r="A13" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="4"/>
-      <c r="C13" s="10"/>
+      <c r="B13" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>57</v>
+      </c>
       <c r="D13" s="6"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4">
       <c r="A14" s="7" t="s">
         <v>12</v>
       </c>
@@ -766,7 +775,7 @@
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4">
       <c r="A15" s="7" t="s">
         <v>15</v>
       </c>
@@ -774,7 +783,7 @@
       <c r="C15" s="4"/>
       <c r="D15" s="6"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4">
       <c r="A16" s="7" t="s">
         <v>16</v>
       </c>
@@ -782,7 +791,7 @@
       <c r="C16" s="5"/>
       <c r="D16" s="6"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4">
       <c r="A17" s="7" t="s">
         <v>17</v>
       </c>
@@ -790,7 +799,7 @@
       <c r="C17" s="6"/>
       <c r="D17" s="6"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4">
       <c r="A18" s="7" t="s">
         <v>18</v>
       </c>
@@ -798,7 +807,7 @@
       <c r="C18" s="6"/>
       <c r="D18" s="6"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4">
       <c r="A19" s="7" t="s">
         <v>20</v>
       </c>
@@ -806,7 +815,7 @@
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4">
       <c r="A20" s="7" t="s">
         <v>21</v>
       </c>
@@ -814,7 +823,7 @@
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4">
       <c r="A21" s="7" t="s">
         <v>22</v>
       </c>
@@ -822,7 +831,7 @@
       <c r="C21" s="4"/>
       <c r="D21" s="5"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4">
       <c r="A22" s="7" t="s">
         <v>23</v>
       </c>
@@ -830,7 +839,7 @@
       <c r="C22" s="6"/>
       <c r="D22" s="6"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4">
       <c r="A23" s="7" t="s">
         <v>24</v>
       </c>
@@ -838,7 +847,7 @@
       <c r="C23" s="6"/>
       <c r="D23" s="6"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4">
       <c r="A24" s="7" t="s">
         <v>25</v>
       </c>
@@ -846,7 +855,7 @@
       <c r="C24" s="6"/>
       <c r="D24" s="6"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4">
       <c r="A26" s="7"/>
       <c r="B26" s="8" t="s">
         <v>19</v>
@@ -855,7 +864,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4">
       <c r="A27" s="7" t="s">
         <v>27</v>
       </c>
@@ -866,7 +875,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4">
       <c r="A28" s="7" t="s">
         <v>28</v>
       </c>
@@ -877,7 +886,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4">
       <c r="A29" s="7" t="s">
         <v>29</v>
       </c>
@@ -888,7 +897,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4">
       <c r="A30" s="7" t="s">
         <v>30</v>
       </c>
@@ -899,7 +908,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4">
       <c r="A31" s="7" t="s">
         <v>31</v>
       </c>
@@ -910,7 +919,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4">
       <c r="A32" s="7" t="s">
         <v>32</v>
       </c>
@@ -921,7 +930,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3">
       <c r="A33" s="7" t="s">
         <v>33</v>
       </c>
@@ -932,32 +941,38 @@
         <v>53</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3">
       <c r="A34" s="7" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B34" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C34" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
       <c r="A35" s="7" t="s">
         <v>35</v>
       </c>
       <c r="B35" s="6"/>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3">
       <c r="A36" s="7" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3">
       <c r="B37" s="5"/>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3">
       <c r="B38" s="6"/>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3">
       <c r="B39" s="4"/>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3">
       <c r="B40" s="5"/>
     </row>
   </sheetData>
@@ -972,12 +987,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -989,12 +1004,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>